<commit_message>
Brief 5 Requirements (1)
</commit_message>
<xml_diff>
--- a/AGA307 Programming Assessment 1 Checklist.xlsx
+++ b/AGA307 Programming Assessment 1 Checklist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/519cb0034a3fc690/UNI/AGA307 - Game Dev II - Programming/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jskinner2\Workspace\Skinner_J_AGA307_Assessment-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -507,7 +507,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$I$35" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$I$35" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -515,15 +515,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$I$36" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$I$36" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$I$37" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$I$37" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$I$38" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$I$38" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
@@ -531,7 +531,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$I$41" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$I$41" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
@@ -543,11 +543,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$I$47" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$I$47" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp28.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$I$48" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$I$48" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3333,7 +3333,7 @@
       </c>
       <c r="N7" s="12">
         <f>COUNTIFS(I4:I64,TRUE,J4:J64,"Required")</f>
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3351,7 +3351,7 @@
       </c>
       <c r="N8" s="13">
         <f>COUNTIFS(I4:I64,TRUE,J4:J64,"Required")/COUNTIFS(I4:I64,"&lt;&gt;",J4:J64,"Required")</f>
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="9" spans="2:14" ht="25.5" x14ac:dyDescent="0.2">
@@ -3398,7 +3398,7 @@
       </c>
       <c r="N10" s="12">
         <f>COUNTIFS(I4:I64,TRUE,J4:J64,"Challenge")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.2">
@@ -3413,7 +3413,7 @@
       </c>
       <c r="N11" s="13">
         <f>COUNTIFS(I4:I64,TRUE,J4:J64,"Challenge")/COUNTIFS(I4:I64,"&lt;&gt;",J4:J64,"Challenge")</f>
-        <v>0.125</v>
+        <v>0.1875</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.2">
@@ -3774,11 +3774,11 @@
       <c r="D35" s="11"/>
       <c r="E35" s="11" t="str">
         <f>IF(I35,"Done","To Be Done")</f>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="F35" s="24"/>
       <c r="I35" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J35" s="9" t="s">
         <v>4</v>
@@ -3794,11 +3794,11 @@
       <c r="D36" s="11"/>
       <c r="E36" s="11" t="str">
         <f>IF(I36,"Done","To Be Done")</f>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="F36" s="24"/>
       <c r="I36" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J36" s="9" t="s">
         <v>4</v>
@@ -3814,11 +3814,11 @@
       <c r="D37" s="11"/>
       <c r="E37" s="11" t="str">
         <f>IF(I37,"Done","To Be Done")</f>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="F37" s="24"/>
       <c r="I37" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J37" s="9" t="s">
         <v>4</v>
@@ -3834,11 +3834,11 @@
       <c r="D38" s="11"/>
       <c r="E38" s="11" t="str">
         <f>IF(I38,"Done","To Be Done")</f>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="F38" s="24"/>
       <c r="I38" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38" s="9" t="s">
         <v>4</v>
@@ -3885,11 +3885,11 @@
       <c r="D41" s="11"/>
       <c r="E41" s="11" t="str">
         <f>IF(I41,"Done","To Be Done")</f>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="F41" s="24"/>
       <c r="I41" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J41" s="9" t="s">
         <v>47</v>
@@ -3971,11 +3971,11 @@
       <c r="D47" s="11"/>
       <c r="E47" s="11" t="str">
         <f>IF(I47,"Done","To Be Done")</f>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="F47" s="24"/>
       <c r="I47" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J47" s="9" t="s">
         <v>4</v>
@@ -3991,11 +3991,11 @@
       <c r="D48" s="11"/>
       <c r="E48" s="11" t="str">
         <f>IF(I48,"Done","To Be Done")</f>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="F48" s="24"/>
       <c r="I48" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J48" s="9" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Brief 5 Requirements (2)
</commit_message>
<xml_diff>
--- a/AGA307 Programming Assessment 1 Checklist.xlsx
+++ b/AGA307 Programming Assessment 1 Checklist.xlsx
@@ -1,30 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jskinner2\Workspace\Skinner_J_AGA307_Assessment-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\GitHub\Skinner_J_AGA307_Assessment-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E17C2F-FB75-4473-BE7C-A825918273A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="57">
   <si>
     <t>Status</t>
   </si>
@@ -192,16 +204,19 @@
   </si>
   <si>
     <t>Jackson Skinner</t>
+  </si>
+  <si>
+    <t>https://github.com/Valgius/Skinner_J_AGA307_Assessment-1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -231,6 +246,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -329,10 +351,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -344,7 +367,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -354,7 +377,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -368,22 +390,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -408,8 +427,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
@@ -551,7 +575,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$I$49" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$I$49" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -634,6 +658,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1035"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -698,6 +725,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1036"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -762,6 +792,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1037"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -826,6 +859,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1038"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -890,6 +926,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1040"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -954,6 +993,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1041"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1018,6 +1060,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1054"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1082,6 +1127,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1055"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1146,6 +1194,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1056"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1210,6 +1261,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1057"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1274,6 +1328,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1059"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1338,6 +1395,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1060"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1402,6 +1462,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1062"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1466,6 +1529,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1063"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1530,6 +1596,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1065"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1594,6 +1663,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1066"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002A040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1658,6 +1730,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1067"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002B040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1722,6 +1797,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1068"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1786,6 +1864,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1070"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1850,6 +1931,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1071"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002F040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1914,6 +1998,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1072"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000030040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -1978,6 +2065,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1073"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000031040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -2042,6 +2132,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1075"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000033040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -2106,6 +2199,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1076"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000034040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -2170,6 +2266,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1077"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000035040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -2234,6 +2333,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1078"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000036040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -2298,6 +2400,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1080"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000038040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -2362,6 +2467,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1081"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000039040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -2426,6 +2534,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1082"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003A040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -2490,6 +2601,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1085"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003D040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -2554,6 +2668,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1086"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003E040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -2618,6 +2735,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1090"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000042040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -2682,6 +2802,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1091"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000043040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -2746,6 +2869,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1092"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000044040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -2810,6 +2936,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1095"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000047040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -2873,6 +3002,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1096"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000048040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3181,21 +3313,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:N61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="C1" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1.875" style="3" customWidth="1"/>
     <col min="2" max="2" width="6.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.875" style="21" customWidth="1"/>
+    <col min="3" max="3" width="53.875" style="18" customWidth="1"/>
     <col min="4" max="4" width="7.625" style="3" customWidth="1"/>
     <col min="5" max="5" width="11.75" style="3" customWidth="1"/>
-    <col min="6" max="6" width="32.875" style="21" customWidth="1"/>
+    <col min="6" max="6" width="32.875" style="18" customWidth="1"/>
     <col min="7" max="7" width="1.75" style="3" customWidth="1"/>
     <col min="8" max="8" width="1.75" style="3" hidden="1" customWidth="1"/>
     <col min="9" max="10" width="10.875" style="3" hidden="1" customWidth="1"/>
@@ -3210,14 +3342,14 @@
       <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="17"/>
+      <c r="D2" s="16"/>
       <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="20" t="s">
         <v>50</v>
       </c>
       <c r="I2" s="4" t="s">
@@ -3229,983 +3361,963 @@
       </c>
     </row>
     <row r="3" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="28"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="26"/>
       <c r="I3" s="8"/>
-      <c r="J3" s="9"/>
     </row>
     <row r="4" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>1</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11" t="str">
+      <c r="D4" s="10"/>
+      <c r="E4" s="10" t="str">
         <f>IF(I4,"Done","To Be Done")</f>
         <v>Done</v>
       </c>
-      <c r="F4" s="24"/>
+      <c r="F4" s="22"/>
       <c r="I4" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="M4" s="11" t="s">
+      <c r="M4" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="N4" s="23" t="s">
+      <c r="N4" s="21" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="5" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>2</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11" t="str">
+      <c r="D5" s="10"/>
+      <c r="E5" s="10" t="str">
         <f>IF(I5,"Done","To Be Done")</f>
         <v>Done</v>
       </c>
-      <c r="F5" s="24"/>
+      <c r="F5" s="22"/>
       <c r="I5" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="11" t="s">
+      <c r="M5" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="N5" s="23"/>
+      <c r="N5" s="27" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="6" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>3</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11" t="str">
+      <c r="D6" s="10"/>
+      <c r="E6" s="10" t="str">
         <f>IF(I6,"Done","To Be Done")</f>
         <v>Done</v>
       </c>
-      <c r="F6" s="24"/>
+      <c r="F6" s="22"/>
       <c r="I6" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <v>4</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11" t="str">
+      <c r="D7" s="10"/>
+      <c r="E7" s="10" t="str">
         <f>IF(I7,"Done","To Be Done")</f>
         <v>Done</v>
       </c>
-      <c r="F7" s="24"/>
+      <c r="F7" s="22"/>
       <c r="I7" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="M7" s="11" t="s">
+      <c r="M7" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="N7" s="12">
+      <c r="N7" s="11">
         <f>COUNTIFS(I4:I64,TRUE,J4:J64,"Required")</f>
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="28"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="26"/>
       <c r="I8" s="8"/>
-      <c r="J8" s="9"/>
-      <c r="M8" s="11" t="s">
+      <c r="M8" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="N8" s="13">
+      <c r="N8" s="12">
         <f>COUNTIFS(I4:I64,TRUE,J4:J64,"Required")/COUNTIFS(I4:I64,"&lt;&gt;",J4:J64,"Required")</f>
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="9" spans="2:14" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B9" s="10">
+      <c r="B9" s="9">
         <v>1</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11" t="str">
+      <c r="D9" s="10"/>
+      <c r="E9" s="10" t="str">
         <f>IF(I9,"Done","To Be Done")</f>
         <v>To Be Done</v>
       </c>
-      <c r="F9" s="24"/>
+      <c r="F9" s="22"/>
       <c r="I9" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J9" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B10" s="10">
+      <c r="B10" s="9">
         <v>2</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11" t="str">
+      <c r="D10" s="10"/>
+      <c r="E10" s="10" t="str">
         <f>IF(I10,"Done","To Be Done")</f>
         <v>Done</v>
       </c>
-      <c r="F10" s="24"/>
+      <c r="F10" s="22"/>
       <c r="I10" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="J10" s="9" t="s">
+      <c r="J10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="M10" s="11" t="s">
+      <c r="M10" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="N10" s="12">
+      <c r="N10" s="11">
         <f>COUNTIFS(I4:I64,TRUE,J4:J64,"Challenge")</f>
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B11" s="14"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="M11" s="11" t="s">
+      <c r="B11" s="13"/>
+      <c r="M11" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="N11" s="13">
+      <c r="N11" s="12">
         <f>COUNTIFS(I4:I64,TRUE,J4:J64,"Challenge")/COUNTIFS(I4:I64,"&lt;&gt;",J4:J64,"Challenge")</f>
         <v>0.1875</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B12" s="14"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
+      <c r="B12" s="13"/>
     </row>
     <row r="13" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="25" t="s">
+      <c r="D13" s="15"/>
+      <c r="E13" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="20" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="28"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="26"/>
       <c r="I14" s="8"/>
-      <c r="J14" s="9"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B15" s="10">
+      <c r="B15" s="9">
         <v>1</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11" t="str">
+      <c r="D15" s="10"/>
+      <c r="E15" s="10" t="str">
         <f>IF(I15,"Done","To Be Done")</f>
         <v>Done</v>
       </c>
-      <c r="F15" s="24"/>
+      <c r="F15" s="22"/>
       <c r="I15" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="J15" s="9" t="s">
+      <c r="J15" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B16" s="10">
+      <c r="B16" s="9">
         <v>2</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11" t="str">
+      <c r="D16" s="10"/>
+      <c r="E16" s="10" t="str">
         <f>IF(I16,"Done","To Be Done")</f>
         <v>Done</v>
       </c>
-      <c r="F16" s="24"/>
+      <c r="F16" s="22"/>
       <c r="I16" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="J16" s="9" t="s">
+      <c r="J16" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="10">
+      <c r="B17" s="9">
         <v>3</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11" t="str">
+      <c r="D17" s="10"/>
+      <c r="E17" s="10" t="str">
         <f>IF(I17,"Done","To Be Done")</f>
         <v>Done</v>
       </c>
-      <c r="F17" s="24"/>
+      <c r="F17" s="22"/>
       <c r="I17" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="J17" s="9" t="s">
+      <c r="J17" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B18" s="10">
+      <c r="B18" s="9">
         <v>4</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11" t="str">
+      <c r="D18" s="10"/>
+      <c r="E18" s="10" t="str">
         <f>IF(I18,"Done","To Be Done")</f>
         <v>Done</v>
       </c>
-      <c r="F18" s="24"/>
+      <c r="F18" s="22"/>
       <c r="I18" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="J18" s="9" t="s">
+      <c r="J18" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="28"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="26"/>
       <c r="I19" s="8"/>
-      <c r="J19" s="9"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B20" s="10">
+      <c r="B20" s="9">
         <v>1</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11" t="str">
+      <c r="D20" s="10"/>
+      <c r="E20" s="10" t="str">
         <f>IF(I20,"Done","To Be Done")</f>
         <v>Done</v>
       </c>
-      <c r="F20" s="24"/>
+      <c r="F20" s="22"/>
       <c r="I20" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="J20" s="9" t="s">
+      <c r="J20" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B21" s="10">
+      <c r="B21" s="9">
         <v>2</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11" t="str">
+      <c r="D21" s="10"/>
+      <c r="E21" s="10" t="str">
         <f>IF(I21,"Done","To Be Done")</f>
         <v>To Be Done</v>
       </c>
-      <c r="F21" s="24"/>
+      <c r="F21" s="22"/>
       <c r="I21" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="J21" s="9" t="s">
+      <c r="J21" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="16"/>
-      <c r="E23" s="25" t="s">
+      <c r="D23" s="15"/>
+      <c r="E23" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="F23" s="22" t="s">
+      <c r="F23" s="20" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="28"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="26"/>
       <c r="I24" s="8"/>
-      <c r="J24" s="9"/>
     </row>
     <row r="25" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B25" s="10">
+      <c r="B25" s="9">
         <v>1</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11" t="str">
+      <c r="D25" s="10"/>
+      <c r="E25" s="10" t="str">
         <f>IF(I25,"Done","To Be Done")</f>
         <v>Done</v>
       </c>
-      <c r="F25" s="24"/>
+      <c r="F25" s="22"/>
       <c r="I25" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="J25" s="9" t="s">
+      <c r="J25" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="26" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B26" s="10">
+      <c r="B26" s="9">
         <v>2</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11" t="str">
+      <c r="D26" s="10"/>
+      <c r="E26" s="10" t="str">
         <f>IF(I26,"Done","To Be Done")</f>
         <v>Done</v>
       </c>
-      <c r="F26" s="24"/>
+      <c r="F26" s="22"/>
       <c r="I26" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="J26" s="9" t="s">
+      <c r="J26" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="28"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="26"/>
       <c r="I27" s="8"/>
-      <c r="J27" s="9"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B28" s="10">
+      <c r="B28" s="9">
         <v>1</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11" t="str">
+      <c r="D28" s="10"/>
+      <c r="E28" s="10" t="str">
         <f>IF(I28,"Done","To Be Done")</f>
         <v>To Be Done</v>
       </c>
-      <c r="F28" s="24"/>
+      <c r="F28" s="22"/>
       <c r="I28" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="J28" s="9" t="s">
+      <c r="J28" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B29" s="10">
+      <c r="B29" s="9">
         <v>2</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="C29" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11" t="str">
+      <c r="D29" s="10"/>
+      <c r="E29" s="10" t="str">
         <f>IF(I29,"Done","To Be Done")</f>
         <v>To Be Done</v>
       </c>
-      <c r="F29" s="24"/>
+      <c r="F29" s="22"/>
       <c r="I29" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="J29" s="9" t="s">
+      <c r="J29" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B30" s="10">
+      <c r="B30" s="9">
         <v>3</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11" t="str">
+      <c r="D30" s="10"/>
+      <c r="E30" s="10" t="str">
         <f>IF(I30,"Done","To Be Done")</f>
         <v>To Be Done</v>
       </c>
-      <c r="F30" s="24"/>
+      <c r="F30" s="22"/>
       <c r="I30" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="J30" s="9" t="s">
+      <c r="J30" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B31" s="10">
+      <c r="B31" s="9">
         <v>4</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="C31" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11" t="str">
+      <c r="D31" s="10"/>
+      <c r="E31" s="10" t="str">
         <f>IF(I31,"Done","To Be Done")</f>
         <v>To Be Done</v>
       </c>
-      <c r="F31" s="24"/>
+      <c r="F31" s="22"/>
       <c r="I31" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="J31" s="9" t="s">
+      <c r="J31" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C33" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D33" s="16"/>
-      <c r="E33" s="25" t="s">
+      <c r="D33" s="15"/>
+      <c r="E33" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="F33" s="22" t="s">
+      <c r="F33" s="20" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="28"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="26"/>
       <c r="I34" s="8"/>
-      <c r="J34" s="9"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B35" s="10">
+      <c r="B35" s="9">
         <v>1</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="C35" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11" t="str">
+      <c r="D35" s="10"/>
+      <c r="E35" s="10" t="str">
         <f>IF(I35,"Done","To Be Done")</f>
         <v>Done</v>
       </c>
-      <c r="F35" s="24"/>
+      <c r="F35" s="22"/>
       <c r="I35" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="J35" s="9" t="s">
+      <c r="J35" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="36" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B36" s="10">
+      <c r="B36" s="9">
         <v>2</v>
       </c>
-      <c r="C36" s="18" t="s">
+      <c r="C36" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11" t="str">
+      <c r="D36" s="10"/>
+      <c r="E36" s="10" t="str">
         <f>IF(I36,"Done","To Be Done")</f>
         <v>Done</v>
       </c>
-      <c r="F36" s="24"/>
+      <c r="F36" s="22"/>
       <c r="I36" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="J36" s="9" t="s">
+      <c r="J36" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="37" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B37" s="10">
+      <c r="B37" s="9">
         <v>3</v>
       </c>
-      <c r="C37" s="18" t="s">
+      <c r="C37" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11" t="str">
+      <c r="D37" s="10"/>
+      <c r="E37" s="10" t="str">
         <f>IF(I37,"Done","To Be Done")</f>
         <v>Done</v>
       </c>
-      <c r="F37" s="24"/>
+      <c r="F37" s="22"/>
       <c r="I37" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="J37" s="9" t="s">
+      <c r="J37" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B38" s="10">
+      <c r="B38" s="9">
         <v>4</v>
       </c>
-      <c r="C38" s="18" t="s">
+      <c r="C38" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11" t="str">
+      <c r="D38" s="10"/>
+      <c r="E38" s="10" t="str">
         <f>IF(I38,"Done","To Be Done")</f>
         <v>Done</v>
       </c>
-      <c r="F38" s="24"/>
+      <c r="F38" s="22"/>
       <c r="I38" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="J38" s="9" t="s">
+      <c r="J38" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B39" s="26" t="s">
+      <c r="B39" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="28"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="26"/>
       <c r="I39" s="8"/>
-      <c r="J39" s="9"/>
     </row>
     <row r="40" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B40" s="10">
+      <c r="B40" s="9">
         <v>1</v>
       </c>
-      <c r="C40" s="18" t="s">
+      <c r="C40" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11" t="str">
+      <c r="D40" s="10"/>
+      <c r="E40" s="10" t="str">
         <f>IF(I40,"Done","To Be Done")</f>
         <v>To Be Done</v>
       </c>
-      <c r="F40" s="24"/>
+      <c r="F40" s="22"/>
       <c r="I40" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="J40" s="9" t="s">
+      <c r="J40" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B41" s="10">
+      <c r="B41" s="9">
         <v>2</v>
       </c>
-      <c r="C41" s="18" t="s">
+      <c r="C41" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11" t="str">
+      <c r="D41" s="10"/>
+      <c r="E41" s="10" t="str">
         <f>IF(I41,"Done","To Be Done")</f>
         <v>Done</v>
       </c>
-      <c r="F41" s="24"/>
+      <c r="F41" s="22"/>
       <c r="I41" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="J41" s="9" t="s">
+      <c r="J41" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B42" s="10">
+      <c r="B42" s="9">
         <v>3</v>
       </c>
-      <c r="C42" s="18" t="s">
+      <c r="C42" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11" t="str">
+      <c r="D42" s="10"/>
+      <c r="E42" s="10" t="str">
         <f t="shared" ref="E42:E43" si="0">IF(I42,"Done","To Be Done")</f>
         <v>To Be Done</v>
       </c>
-      <c r="F42" s="24"/>
+      <c r="F42" s="22"/>
       <c r="I42" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="J42" s="9" t="s">
+      <c r="J42" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B43" s="10">
+      <c r="B43" s="9">
         <v>4</v>
       </c>
-      <c r="C43" s="18" t="s">
+      <c r="C43" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11" t="str">
+      <c r="D43" s="10"/>
+      <c r="E43" s="10" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="F43" s="24"/>
+      <c r="F43" s="22"/>
       <c r="I43" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="J43" s="9" t="s">
+      <c r="J43" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C45" s="20" t="s">
+      <c r="C45" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D45" s="16"/>
-      <c r="E45" s="25" t="s">
+      <c r="D45" s="15"/>
+      <c r="E45" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="F45" s="22" t="s">
+      <c r="F45" s="20" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B46" s="26" t="s">
+      <c r="B46" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C46" s="27"/>
-      <c r="D46" s="27"/>
-      <c r="E46" s="27"/>
-      <c r="F46" s="28"/>
+      <c r="C46" s="25"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="25"/>
+      <c r="F46" s="26"/>
       <c r="I46" s="8"/>
-      <c r="J46" s="9"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B47" s="10">
+      <c r="B47" s="9">
         <v>1</v>
       </c>
-      <c r="C47" s="18" t="s">
+      <c r="C47" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11" t="str">
+      <c r="D47" s="10"/>
+      <c r="E47" s="10" t="str">
         <f>IF(I47,"Done","To Be Done")</f>
         <v>Done</v>
       </c>
-      <c r="F47" s="24"/>
+      <c r="F47" s="22"/>
       <c r="I47" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="J47" s="9" t="s">
+      <c r="J47" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="48" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B48" s="10">
+      <c r="B48" s="9">
         <v>2</v>
       </c>
-      <c r="C48" s="18" t="s">
+      <c r="C48" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11" t="str">
+      <c r="D48" s="10"/>
+      <c r="E48" s="10" t="str">
         <f>IF(I48,"Done","To Be Done")</f>
         <v>Done</v>
       </c>
-      <c r="F48" s="24"/>
+      <c r="F48" s="22"/>
       <c r="I48" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="J48" s="9" t="s">
+      <c r="J48" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="49" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B49" s="10">
+      <c r="B49" s="9">
         <v>3</v>
       </c>
-      <c r="C49" s="18" t="s">
+      <c r="C49" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11" t="str">
+      <c r="D49" s="10"/>
+      <c r="E49" s="10" t="str">
         <f>IF(I49,"Done","To Be Done")</f>
-        <v>To Be Done</v>
-      </c>
-      <c r="F49" s="24"/>
+        <v>Done</v>
+      </c>
+      <c r="F49" s="22"/>
       <c r="I49" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="J49" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J49" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B50" s="26" t="s">
+      <c r="B50" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C50" s="27"/>
-      <c r="D50" s="27"/>
-      <c r="E50" s="27"/>
-      <c r="F50" s="28"/>
+      <c r="C50" s="25"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="26"/>
       <c r="I50" s="8"/>
-      <c r="J50" s="9"/>
     </row>
     <row r="51" spans="2:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B51" s="10">
+      <c r="B51" s="9">
         <v>1</v>
       </c>
-      <c r="C51" s="18" t="s">
+      <c r="C51" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11" t="str">
+      <c r="D51" s="10"/>
+      <c r="E51" s="10" t="str">
         <f>IF(I51,"Done","To Be Done")</f>
         <v>To Be Done</v>
       </c>
-      <c r="F51" s="24"/>
+      <c r="F51" s="22"/>
       <c r="I51" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="J51" s="9" t="s">
+      <c r="J51" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="52" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B52" s="10">
+      <c r="B52" s="9">
         <v>2</v>
       </c>
-      <c r="C52" s="18" t="s">
+      <c r="C52" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D52" s="11"/>
-      <c r="E52" s="11" t="str">
+      <c r="D52" s="10"/>
+      <c r="E52" s="10" t="str">
         <f>IF(I52,"Done","To Be Done")</f>
         <v>To Be Done</v>
       </c>
-      <c r="F52" s="24"/>
+      <c r="F52" s="22"/>
       <c r="I52" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="J52" s="9" t="s">
+      <c r="J52" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B54" s="15" t="s">
+      <c r="B54" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C54" s="20" t="s">
+      <c r="C54" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="D54" s="16"/>
-      <c r="E54" s="25" t="s">
+      <c r="D54" s="15"/>
+      <c r="E54" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="F54" s="22" t="s">
+      <c r="F54" s="20" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B55" s="26" t="s">
+      <c r="B55" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
-      <c r="E55" s="27"/>
-      <c r="F55" s="28"/>
+      <c r="C55" s="25"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="25"/>
+      <c r="F55" s="26"/>
       <c r="I55" s="8"/>
-      <c r="J55" s="9"/>
     </row>
     <row r="56" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B56" s="10">
+      <c r="B56" s="9">
         <v>1</v>
       </c>
-      <c r="C56" s="18" t="s">
+      <c r="C56" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D56" s="11"/>
-      <c r="E56" s="11" t="str">
+      <c r="D56" s="10"/>
+      <c r="E56" s="10" t="str">
         <f>IF(I56,"Done","To Be Done")</f>
         <v>To Be Done</v>
       </c>
-      <c r="F56" s="24"/>
+      <c r="F56" s="22"/>
       <c r="I56" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="J56" s="9" t="s">
+      <c r="J56" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="57" spans="2:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B57" s="10">
+      <c r="B57" s="9">
         <v>2</v>
       </c>
-      <c r="C57" s="18" t="s">
+      <c r="C57" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D57" s="11"/>
-      <c r="E57" s="11" t="str">
+      <c r="D57" s="10"/>
+      <c r="E57" s="10" t="str">
         <f>IF(I57,"Done","To Be Done")</f>
         <v>To Be Done</v>
       </c>
-      <c r="F57" s="24"/>
+      <c r="F57" s="22"/>
       <c r="I57" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="J57" s="9" t="s">
+      <c r="J57" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="58" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B58" s="10">
+      <c r="B58" s="9">
         <v>3</v>
       </c>
-      <c r="C58" s="18" t="s">
+      <c r="C58" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D58" s="11"/>
-      <c r="E58" s="11" t="str">
+      <c r="D58" s="10"/>
+      <c r="E58" s="10" t="str">
         <f>IF(I58,"Done","To Be Done")</f>
         <v>To Be Done</v>
       </c>
-      <c r="F58" s="24"/>
+      <c r="F58" s="22"/>
       <c r="I58" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="J58" s="9" t="s">
+      <c r="J58" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B59" s="26" t="s">
+      <c r="B59" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C59" s="27"/>
-      <c r="D59" s="27"/>
-      <c r="E59" s="27"/>
-      <c r="F59" s="28"/>
+      <c r="C59" s="25"/>
+      <c r="D59" s="25"/>
+      <c r="E59" s="25"/>
+      <c r="F59" s="26"/>
       <c r="I59" s="8"/>
-      <c r="J59" s="9"/>
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B60" s="10">
+      <c r="B60" s="9">
         <v>1</v>
       </c>
-      <c r="C60" s="18" t="s">
+      <c r="C60" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D60" s="11"/>
-      <c r="E60" s="11" t="str">
+      <c r="D60" s="10"/>
+      <c r="E60" s="10" t="str">
         <f>IF(I60,"Done","To Be Done")</f>
         <v>To Be Done</v>
       </c>
-      <c r="F60" s="24"/>
+      <c r="F60" s="22"/>
       <c r="I60" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="J60" s="9" t="s">
+      <c r="J60" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="61" spans="2:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B61" s="10">
+      <c r="B61" s="9">
         <v>2</v>
       </c>
-      <c r="C61" s="18" t="s">
+      <c r="C61" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11" t="str">
+      <c r="D61" s="10"/>
+      <c r="E61" s="10" t="str">
         <f>IF(I61,"Done","To Be Done")</f>
         <v>To Be Done</v>
       </c>
-      <c r="F61" s="24"/>
+      <c r="F61" s="22"/>
       <c r="I61" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="J61" s="9" t="s">
+      <c r="J61" s="3" t="s">
         <v>47</v>
       </c>
     </row>
@@ -4224,7 +4336,7 @@
     <mergeCell ref="B46:F46"/>
     <mergeCell ref="B50:F50"/>
   </mergeCells>
-  <conditionalFormatting sqref="E4:E7 E47:E49 E56:E58 E9:E12 E51:E52 E60:E61">
+  <conditionalFormatting sqref="E4:E7 E9:E12 E47:E49 E51:E52 E56:E58 E60:E61">
     <cfRule type="expression" dxfId="3" priority="7">
       <formula>$E4="Done"</formula>
     </cfRule>
@@ -4244,16 +4356,19 @@
       <formula>$E35="Done"</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="N5" r:id="rId1" xr:uid="{AD08B9FE-4B85-419E-9F4F-F75F9483C8EF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup paperSize="8" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x14">
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1035" r:id="rId4" name="Check Box 11">
+            <control shapeId="1035" r:id="rId5" name="Check Box 11">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4275,7 +4390,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1036" r:id="rId5" name="Check Box 12">
+            <control shapeId="1036" r:id="rId6" name="Check Box 12">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4297,7 +4412,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1037" r:id="rId6" name="Check Box 13">
+            <control shapeId="1037" r:id="rId7" name="Check Box 13">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4319,7 +4434,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1038" r:id="rId7" name="Check Box 14">
+            <control shapeId="1038" r:id="rId8" name="Check Box 14">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4341,7 +4456,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1040" r:id="rId8" name="Check Box 16">
+            <control shapeId="1040" r:id="rId9" name="Check Box 16">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4363,7 +4478,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1041" r:id="rId9" name="Check Box 17">
+            <control shapeId="1041" r:id="rId10" name="Check Box 17">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4385,7 +4500,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1054" r:id="rId10" name="Check Box 30">
+            <control shapeId="1054" r:id="rId11" name="Check Box 30">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4407,7 +4522,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1055" r:id="rId11" name="Check Box 31">
+            <control shapeId="1055" r:id="rId12" name="Check Box 31">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4429,7 +4544,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1056" r:id="rId12" name="Check Box 32">
+            <control shapeId="1056" r:id="rId13" name="Check Box 32">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4451,7 +4566,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1057" r:id="rId13" name="Check Box 33">
+            <control shapeId="1057" r:id="rId14" name="Check Box 33">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4473,7 +4588,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1059" r:id="rId14" name="Check Box 35">
+            <control shapeId="1059" r:id="rId15" name="Check Box 35">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4495,7 +4610,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1060" r:id="rId15" name="Check Box 36">
+            <control shapeId="1060" r:id="rId16" name="Check Box 36">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4517,7 +4632,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1062" r:id="rId16" name="Check Box 38">
+            <control shapeId="1062" r:id="rId17" name="Check Box 38">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4539,7 +4654,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1063" r:id="rId17" name="Check Box 39">
+            <control shapeId="1063" r:id="rId18" name="Check Box 39">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4561,7 +4676,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1065" r:id="rId18" name="Check Box 41">
+            <control shapeId="1065" r:id="rId19" name="Check Box 41">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4583,7 +4698,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1066" r:id="rId19" name="Check Box 42">
+            <control shapeId="1066" r:id="rId20" name="Check Box 42">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4605,7 +4720,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1067" r:id="rId20" name="Check Box 43">
+            <control shapeId="1067" r:id="rId21" name="Check Box 43">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4627,7 +4742,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1068" r:id="rId21" name="Check Box 44">
+            <control shapeId="1068" r:id="rId22" name="Check Box 44">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4649,7 +4764,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1070" r:id="rId22" name="Check Box 46">
+            <control shapeId="1070" r:id="rId23" name="Check Box 46">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4671,7 +4786,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1071" r:id="rId23" name="Check Box 47">
+            <control shapeId="1071" r:id="rId24" name="Check Box 47">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4693,7 +4808,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1072" r:id="rId24" name="Check Box 48">
+            <control shapeId="1072" r:id="rId25" name="Check Box 48">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4715,7 +4830,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1073" r:id="rId25" name="Check Box 49">
+            <control shapeId="1073" r:id="rId26" name="Check Box 49">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4737,7 +4852,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1075" r:id="rId26" name="Check Box 51">
+            <control shapeId="1075" r:id="rId27" name="Check Box 51">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4759,7 +4874,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1076" r:id="rId27" name="Check Box 52">
+            <control shapeId="1076" r:id="rId28" name="Check Box 52">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4781,7 +4896,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1077" r:id="rId28" name="Check Box 53">
+            <control shapeId="1077" r:id="rId29" name="Check Box 53">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4803,7 +4918,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1078" r:id="rId29" name="Check Box 54">
+            <control shapeId="1078" r:id="rId30" name="Check Box 54">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4825,7 +4940,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1080" r:id="rId30" name="Check Box 56">
+            <control shapeId="1080" r:id="rId31" name="Check Box 56">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4847,7 +4962,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1081" r:id="rId31" name="Check Box 57">
+            <control shapeId="1081" r:id="rId32" name="Check Box 57">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4869,7 +4984,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1082" r:id="rId32" name="Check Box 58">
+            <control shapeId="1082" r:id="rId33" name="Check Box 58">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4891,7 +5006,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1085" r:id="rId33" name="Check Box 61">
+            <control shapeId="1085" r:id="rId34" name="Check Box 61">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4913,7 +5028,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1086" r:id="rId34" name="Check Box 62">
+            <control shapeId="1086" r:id="rId35" name="Check Box 62">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4935,7 +5050,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1090" r:id="rId35" name="Check Box 66">
+            <control shapeId="1090" r:id="rId36" name="Check Box 66">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4957,7 +5072,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1091" r:id="rId36" name="Check Box 67">
+            <control shapeId="1091" r:id="rId37" name="Check Box 67">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4979,7 +5094,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1092" r:id="rId37" name="Check Box 68">
+            <control shapeId="1092" r:id="rId38" name="Check Box 68">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5001,7 +5116,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1095" r:id="rId38" name="Check Box 71">
+            <control shapeId="1095" r:id="rId39" name="Check Box 71">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5023,7 +5138,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1096" r:id="rId39" name="Check Box 72">
+            <control shapeId="1096" r:id="rId40" name="Check Box 72">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>

</xml_diff>

<commit_message>
Brief 4 Challenges (1) 1-3 Complete. 4 Attempt.
</commit_message>
<xml_diff>
--- a/AGA307 Programming Assessment 1 Checklist.xlsx
+++ b/AGA307 Programming Assessment 1 Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\GitHub\Skinner_J_AGA307_Assessment-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA33C4D7-E82F-416D-9B6E-AC76116CE599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1581187A-5179-402C-8002-39347D2CCC04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19080" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -551,7 +551,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$I$40" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$I$40" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
@@ -559,7 +559,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$I$42" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$I$42" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3316,8 +3316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:N61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="C13" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="C31" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3530,7 +3530,7 @@
       </c>
       <c r="N10" s="11">
         <f>COUNTIFS(I4:I64,TRUE,J4:J64,"Challenge")</f>
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.2">
@@ -3540,7 +3540,7 @@
       </c>
       <c r="N11" s="12">
         <f>COUNTIFS(I4:I64,TRUE,J4:J64,"Challenge")/COUNTIFS(I4:I64,"&lt;&gt;",J4:J64,"Challenge")</f>
-        <v>0.5625</v>
+        <v>0.6875</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.2">
@@ -3981,11 +3981,11 @@
       <c r="D40" s="10"/>
       <c r="E40" s="10" t="str">
         <f>IF(I40,"Done","To Be Done")</f>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="F40" s="22"/>
       <c r="I40" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J40" s="3" t="s">
         <v>47</v>
@@ -4021,11 +4021,11 @@
       <c r="D42" s="10"/>
       <c r="E42" s="10" t="str">
         <f t="shared" ref="E42:E43" si="0">IF(I42,"Done","To Be Done")</f>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="F42" s="22"/>
       <c r="I42" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42" s="3" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Brief 6 Challenges (1) 1 Complete.  2 UI elements in place, targets don't change.
</commit_message>
<xml_diff>
--- a/AGA307 Programming Assessment 1 Checklist.xlsx
+++ b/AGA307 Programming Assessment 1 Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\GitHub\Skinner_J_AGA307_Assessment-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1581187A-5179-402C-8002-39347D2CCC04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB78C36-66B5-42FD-9A9B-007326377165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19080" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -603,7 +603,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp35.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$I$60" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$I$60" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp36.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3316,8 +3316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:N61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="C31" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A51" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="M56" sqref="M56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3530,7 +3530,7 @@
       </c>
       <c r="N10" s="11">
         <f>COUNTIFS(I4:I64,TRUE,J4:J64,"Challenge")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.2">
@@ -3540,7 +3540,7 @@
       </c>
       <c r="N11" s="12">
         <f>COUNTIFS(I4:I64,TRUE,J4:J64,"Challenge")/COUNTIFS(I4:I64,"&lt;&gt;",J4:J64,"Challenge")</f>
-        <v>0.6875</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.2">
@@ -4291,11 +4291,11 @@
       <c r="D60" s="10"/>
       <c r="E60" s="10" t="str">
         <f>IF(I60,"Done","To Be Done")</f>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="F60" s="22"/>
       <c r="I60" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J60" s="3" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Brief 6 Challenges (2). 2 complete. Briefs 4 and 5 Challenges  4 and 2 Attempted.
</commit_message>
<xml_diff>
--- a/AGA307 Programming Assessment 1 Checklist.xlsx
+++ b/AGA307 Programming Assessment 1 Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\GitHub\Skinner_J_AGA307_Assessment-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB78C36-66B5-42FD-9A9B-007326377165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2230BB6D-57EE-47F8-A94E-020DAAB077C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19080" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="59">
   <si>
     <t>Status</t>
   </si>
@@ -207,6 +207,12 @@
   </si>
   <si>
     <t>https://github.com/Valgius/Skinner_J_AGA307_Assessment-1</t>
+  </si>
+  <si>
+    <t>swaped to 4,5,6 to not interfer with weapon choice. Attempted. Required repeated button pressed to change all.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Attempted. Required repeated button pressed to change all.</t>
   </si>
 </sst>
 </file>
@@ -607,7 +613,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp36.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$I$61" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$I$61" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2323,8 +2329,8 @@
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>476250</xdr:colOff>
-          <xdr:row>43</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:row>42</xdr:row>
+          <xdr:rowOff>190500</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3316,8 +3322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:N61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A51" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="M56" sqref="M56"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A43" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3530,7 +3536,7 @@
       </c>
       <c r="N10" s="11">
         <f>COUNTIFS(I4:I64,TRUE,J4:J64,"Challenge")</f>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.2">
@@ -3540,7 +3546,7 @@
       </c>
       <c r="N11" s="12">
         <f>COUNTIFS(I4:I64,TRUE,J4:J64,"Challenge")/COUNTIFS(I4:I64,"&lt;&gt;",J4:J64,"Challenge")</f>
-        <v>0.75</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.2">
@@ -4031,7 +4037,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B43" s="9">
         <v>4</v>
       </c>
@@ -4043,7 +4049,9 @@
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="F43" s="22"/>
+      <c r="F43" s="22" t="s">
+        <v>58</v>
+      </c>
       <c r="I43" s="8" t="b">
         <v>0</v>
       </c>
@@ -4166,7 +4174,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B52" s="9">
         <v>2</v>
       </c>
@@ -4178,7 +4186,9 @@
         <f>IF(I52,"Done","To Be Done")</f>
         <v>To Be Done</v>
       </c>
-      <c r="F52" s="22"/>
+      <c r="F52" s="22" t="s">
+        <v>57</v>
+      </c>
       <c r="I52" s="8" t="b">
         <v>0</v>
       </c>
@@ -4311,11 +4321,11 @@
       <c r="D61" s="10"/>
       <c r="E61" s="10" t="str">
         <f>IF(I61,"Done","To Be Done")</f>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="F61" s="22"/>
       <c r="I61" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J61" s="3" t="s">
         <v>47</v>
@@ -4930,8 +4940,8 @@
                   <to>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>476250</xdr:colOff>
-                    <xdr:row>43</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:row>42</xdr:row>
+                    <xdr:rowOff>190500</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>